<commit_message>
Updated Global Glider Cal and Ingest sheets
Changed Cal scattering angle to 140 and angular resolution to 1.13,
changed data source on recovered to recovered_host
</commit_message>
<xml_diff>
--- a/GA05MOAS-GL00#/GA05MOAS-GL00#_R0000#_ingest.xlsx
+++ b/GA05MOAS-GL00#/GA05MOAS-GL00#_R0000#_ingest.xlsx
@@ -28,9 +28,6 @@
     <t>data_source</t>
   </si>
   <si>
-    <t>recovered</t>
-  </si>
-  <si>
     <t>DO NOT CHANGE this column</t>
   </si>
   <si>
@@ -83,6 +80,9 @@
       </rPr>
       <t>However, check for anomalies by verifying that each file path is accurate prior to submission.</t>
     </r>
+  </si>
+  <si>
+    <t>recovered_host</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1213,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,77 +1240,77 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>